<commit_message>
Update tab name in this BRIDG Mapping Tag Glossary spreadsheet
</commit_message>
<xml_diff>
--- a/Working Release Artifacts/Release 5.3.1 Working Drafts/BRIDG Mapping Tag Glossary for Mapping SS jpe-20190712.xlsx
+++ b/Working Release Artifacts/Release 5.3.1 Working Drafts/BRIDG Mapping Tag Glossary for Mapping SS jpe-20190712.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie Evans\Documents\BRIDG\BRIDG 5.3.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie Evans\Documents\GitHub\bridg-model\Working Release Artifacts\Release 5.3.1 Working Drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAEE0A2E-7B05-4372-9BC2-7BBBD0A36D8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7857E00-F8A8-4DCD-BF69-CEBDC3118A29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3D45BC95-9F0A-4510-AB29-BBC7AA311C88}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapping Tag Glossary (2)" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapping Tag Glossary" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -559,12 +559,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,6 +585,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -31268,7 +31268,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="11" customWidth="1"/>
+    <col min="1" max="1" width="6" style="9" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="135.5703125" customWidth="1"/>
     <col min="257" max="257" width="6" customWidth="1"/>
@@ -31463,47 +31463,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -31514,541 +31514,541 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+      <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+      <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+      <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
+      <c r="A36" s="4">
         <v>34</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+      <c r="A37" s="4">
         <v>35</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
+      <c r="A38" s="4">
         <v>36</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+      <c r="A39" s="4">
         <v>37</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+      <c r="A40" s="4">
         <v>38</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
+      <c r="A41" s="4">
         <v>39</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
+      <c r="A42" s="4">
         <v>40</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
+      <c r="A43" s="4">
         <v>41</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
+      <c r="A44" s="4">
         <v>42</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
+      <c r="A45" s="4">
         <v>43</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
+      <c r="A46" s="4">
         <v>44</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="6" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
+      <c r="A47" s="4">
         <v>45</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="6">
+      <c r="A48" s="4">
         <v>46</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6">
+      <c r="A49" s="4">
         <v>47</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6">
+      <c r="A50" s="4">
         <v>48</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
+      <c r="A51" s="4">
         <v>49</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="6">
+      <c r="A52" s="4">
         <v>50</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
+      <c r="A53" s="4">
         <v>51</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="6">
+      <c r="A54" s="4">
         <v>52</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="8" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Mapping Tag Glossary
</commit_message>
<xml_diff>
--- a/Working Release Artifacts/Release 5.3.1 Working Drafts/BRIDG Mapping Tag Glossary for Mapping SS jpe-20190712.xlsx
+++ b/Working Release Artifacts/Release 5.3.1 Working Drafts/BRIDG Mapping Tag Glossary for Mapping SS jpe-20190712.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie Evans\Documents\GitHub\bridg-model\Working Release Artifacts\Release 5.3.1 Working Drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7857E00-F8A8-4DCD-BF69-CEBDC3118A29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE66448-A59A-4EB6-9E15-7F96D4429620}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3D45BC95-9F0A-4510-AB29-BBC7AA311C88}"/>
+    <workbookView xWindow="3525" yWindow="600" windowWidth="14070" windowHeight="11445" xr2:uid="{3D45BC95-9F0A-4510-AB29-BBC7AA311C88}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Tag Glossary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t>BRIDG Model Mapping Tag Names Glossary</t>
   </si>
@@ -368,6 +368,12 @@
   <si>
     <t>World Health Organization (clinical trials registry concepts)</t>
   </si>
+  <si>
+    <t>Map:SDTM IGv3.2</t>
+  </si>
+  <si>
+    <t>CDISC Study Data Tabulation Model Implementation Guide version 3.2</t>
+  </si>
 </sst>
 </file>
 
@@ -31259,7 +31265,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E563478-EEBF-488C-A22A-9E91BB513175}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -31980,10 +31986,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -31991,10 +31997,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -32002,10 +32008,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -32013,10 +32019,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -32024,10 +32030,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -32035,20 +32041,31 @@
         <v>51</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>53</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>